<commit_message>
next part, level one done?
</commit_message>
<xml_diff>
--- a/Sources/Rooms/R1_Guardroom/Bludiste.xlsx
+++ b/Sources/Rooms/R1_Guardroom/Bludiste.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Len\RiderProjects\NajdiCestuVen\Sources\Rooms\R1_Guardroom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F6C17EF-9942-4652-BB9E-C5FCD1073215}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36745C0A-1EC6-4B49-910B-999FC2CD2071}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="5490" windowWidth="29040" windowHeight="15840" xr2:uid="{D946F77B-476C-48B9-B4DE-2E2160B6EADC}"/>
+    <workbookView xWindow="-28920" yWindow="-75" windowWidth="29040" windowHeight="15840" xr2:uid="{D946F77B-476C-48B9-B4DE-2E2160B6EADC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="23">
   <si>
     <t>start</t>
   </si>
@@ -51,13 +51,84 @@
   </si>
   <si>
     <t>&lt;-&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  A B C D E F G H I J</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> #####################</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1#  a  #2       m .  #  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> # # # ######### ### #</t>
+  </si>
+  <si>
+    <t>2# #1#.#     #   #  .#</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> # ### #   # #   ### #</t>
+  </si>
+  <si>
+    <t>3# #  b . f# #    k l#</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> # # ###   # #     # #</t>
+  </si>
+  <si>
+    <t>4#  c#    e#      j# #</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ### #     ### #   ###</t>
+  </si>
+  <si>
+    <t>5#      . g#   #. i  #</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> #     #   #   # ### #</t>
+  </si>
+  <si>
+    <t>6#  d  #  h         .#</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> #####################"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF383838"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF00855F"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>Tr</t>
+    </r>
+  </si>
+  <si>
+    <t>pravda</t>
+  </si>
+  <si>
+    <t>lež</t>
+  </si>
+  <si>
+    <t>nepoužívat</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -66,8 +137,26 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF8C6C41"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF383838"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF00855F"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -86,6 +175,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="22">
     <border>
@@ -326,7 +421,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -419,6 +514,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -734,118 +835,267 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3487372-D723-4284-981C-C6F0F2832539}">
-  <dimension ref="B3:K9"/>
+  <dimension ref="A1:V22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="R19" sqref="R19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="2:11" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="14"/>
-      <c r="C4" s="12" t="s">
+    <row r="1" spans="1:22" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="14"/>
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="26" t="s">
+      <c r="C1" s="7"/>
+      <c r="D1" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="12" t="s">
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="J4" s="32"/>
-      <c r="K4" s="1"/>
-    </row>
-    <row r="5" spans="2:11" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="15"/>
-      <c r="C5" s="13" t="s">
+      <c r="I1" s="32"/>
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:22" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="15"/>
+      <c r="B2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="27"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="31"/>
-    </row>
-    <row r="6" spans="2:11" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="16"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="9" t="s">
+      <c r="C2" s="27"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="31"/>
+    </row>
+    <row r="3" spans="1:22" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="16"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="28"/>
-      <c r="F6" s="18" t="s">
+      <c r="D3" s="28"/>
+      <c r="E3" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="18"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19" t="s">
+      <c r="F3" s="18"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="K6" s="4" t="s">
+      <c r="J3" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="2:11" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="17"/>
-      <c r="C7" s="18" t="s">
+      <c r="N3" s="33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="17"/>
+      <c r="B4" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="19"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="18" t="s">
+      <c r="C4" s="19"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="G7" s="24"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="18" t="s">
+      <c r="F4" s="24"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="K7" s="11"/>
-    </row>
-    <row r="8" spans="2:11" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="2"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="8" t="s">
+      <c r="J4" s="11"/>
+      <c r="N4" s="34" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="G8" s="3"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="29"/>
-      <c r="J8" s="9" t="s">
+      <c r="F5" s="3"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="K8" s="4"/>
-    </row>
-    <row r="9" spans="2:11" ht="49.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="5"/>
-      <c r="C9" s="20" t="s">
+      <c r="J5" s="4"/>
+      <c r="N5" s="34" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" ht="49.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="5"/>
+      <c r="B6" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="21"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6" t="s">
+      <c r="C6" s="21"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="30"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="30"/>
+      <c r="N6" s="34" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="N7" s="34" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="N8" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="T8">
+        <v>1</v>
+      </c>
+      <c r="U8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="D9" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="N9" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="T9">
+        <v>2</v>
+      </c>
+      <c r="U9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="D10" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="N10" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="T10">
+        <v>3</v>
+      </c>
+      <c r="U10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="D11" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="N11" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="T11">
+        <v>4</v>
+      </c>
+      <c r="U11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="D12" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="N12" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="T12">
+        <v>5</v>
+      </c>
+      <c r="U12" t="s">
+        <v>20</v>
+      </c>
+      <c r="V12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="D13" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="N13" s="34" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="D14" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="N14" s="34" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="D15" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="N15" s="34" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="D16" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="N16" s="34" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D17" s="34" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D18" s="34" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D19" s="34" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D20" s="34" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D21" s="34" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D22" s="34" t="s">
+        <v>19</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>